<commit_message>
feat：update battleworld level pre change
</commit_message>
<xml_diff>
--- a/battleworld/Excel/Area_区域表.xlsx
+++ b/battleworld/Excel/Area_区域表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="11775"/>
+    <workbookView windowWidth="24045" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,18 +105,10 @@
     <t>Language</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <charset val="134"/>
-      </rPr>
-      <t>battal_world_nameLV_20</t>
-    </r>
-  </si>
-  <si>
-    <t>211283|22022|2891</t>
+    <t>battal_world_nameLV_20</t>
+  </si>
+  <si>
+    <t>231146|18953|3034</t>
   </si>
   <si>
     <t>0|0|70</t>
@@ -133,7 +125,7 @@
     </r>
   </si>
   <si>
-    <t>216479|-8159|35170</t>
+    <t>212355|18550.12|2758.65</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1111,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" outlineLevelRow="6"/>

</xml_diff>